<commit_message>
Fixed bug in McCormick implementation, stable w free affine responses.
</commit_message>
<xml_diff>
--- a/CS1_24bus/data/24el_12ng/24EL_12NG_Data.xlsx
+++ b/CS1_24bus/data/24el_12ng/24EL_12NG_Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10307"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2C4C1C-E1BE-4373-BD30-CFBEA81F18EE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC596063-A4F9-604B-9D2A-D8C00F658FF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1400" yWindow="460" windowWidth="22260" windowHeight="12640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PowerUnitData" sheetId="1" r:id="rId1"/>
@@ -582,22 +582,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.59765625" customWidth="1"/>
-    <col min="4" max="4" width="7.46484375" customWidth="1"/>
-    <col min="5" max="5" width="8.265625" customWidth="1"/>
-    <col min="7" max="7" width="29.86328125" customWidth="1"/>
-    <col min="8" max="8" width="26.06640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.5" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29.83203125" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -623,7 +623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -650,7 +650,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -677,7 +677,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -704,7 +704,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -731,7 +731,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -758,7 +758,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -785,7 +785,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -812,7 +812,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -839,7 +839,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -866,7 +866,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -893,7 +893,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -920,7 +920,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -947,7 +947,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -955,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>1</v>
       </c>
@@ -963,7 +963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>2</v>
       </c>
@@ -971,7 +971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
@@ -979,7 +979,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -987,7 +987,7 @@
         <v>0.8666666666666667</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>2</v>
       </c>
@@ -995,7 +995,7 @@
         <v>0.8666666666666667</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>3</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>0.78333333333333333</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>4</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>5</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>0.76666666666666672</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>6</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>0.61333333333333329</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>7</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>8</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>0.36666666666666664</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>9</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>0.28333333333333333</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>10</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>0.78333333333333333</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>11</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>0.73333333333333328</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>12</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>0.28333333333333333</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>13</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>0.23333333333333334</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>14</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>15</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>0.28333333333333333</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>16</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>0.68333333333333335</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>17</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>18</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>19</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>0.13333333333333333</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>20</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>21</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>0.11666666666666667</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>22</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>0.11666666666666667</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>23</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>0.6333333333333333</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>24</v>
       </c>
@@ -1184,15 +1184,15 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1273,17 +1273,17 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1328125" style="2"/>
+    <col min="1" max="1" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" style="2"/>
     <col min="5" max="5" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1328125" style="2"/>
+    <col min="6" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1891,20 +1891,20 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="2"/>
-    <col min="2" max="2" width="18.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="2"/>
+    <col min="2" max="2" width="18.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1328125" style="2"/>
+    <col min="5" max="5" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>39300</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>39300</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>49300</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>59300</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>54300</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>54300</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>39300</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>44300</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>39300</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>39300</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>39300</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>29300</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>101</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>102</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>103</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>104</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>105</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>106</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>107</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>108</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>109</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>110</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>111</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>112</v>
       </c>
@@ -2398,13 +2398,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1328125" style="2"/>
+    <col min="1" max="1" width="31.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>2437.5862995382799</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>6700</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>4</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>5</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>6</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>7</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>8</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>9</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>10</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>11</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>12</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>13</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>14</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>15</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>16</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>17</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>1</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>2</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>3</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>4</v>
       </c>
@@ -2897,9 +2897,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="121" zoomScaleNormal="121" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>